<commit_message>
Ajout message à une liste
</commit_message>
<xml_diff>
--- a/Fonctionnalité.xlsx
+++ b/Fonctionnalité.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Desktop\GitHub\S3D_MyWishList\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eddy\git\S3D_MyWishList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3CDE65-1C11-41A5-9AD9-9678FDD0BB05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{3C1348B2-64AF-4800-893C-AA293273578B}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="49">
   <si>
     <t>Fonctionnalite</t>
   </si>
@@ -178,12 +177,15 @@
   </si>
   <si>
     <t>Joindre des listes a son compte</t>
+  </si>
+  <si>
+    <t>newMessage{}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -581,11 +583,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D9E9D4-3346-4702-AFC0-0D490F40261E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,6 +738,9 @@
       <c r="D9" t="s">
         <v>6</v>
       </c>
+      <c r="E9" t="s">
+        <v>48</v>
+      </c>
       <c r="F9">
         <v>3</v>
       </c>

</xml_diff>